<commit_message>
Arrange file operation PRAQuote
</commit_message>
<xml_diff>
--- a/PurchaseRequestApproval/wwwroot/files/tmp/pratmp_3.xlsx
+++ b/PurchaseRequestApproval/wwwroot/files/tmp/pratmp_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ME\C#\Projects\PurchaseRequestApproval\PurchaseRequestApproval\wwwroot\files\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422542FD-8762-41F3-A56B-6BB831B87516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B2BB9E-1EA1-4F90-B49C-CB9093B99C7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1122,7 +1122,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1137,19 +1137,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1805,7 +1793,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1873,27 +1861,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1901,22 +1868,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1942,103 +1893,10 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -2052,22 +1910,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="3" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="3" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2086,46 +1928,22 @@
     <xf numFmtId="165" fontId="11" fillId="0" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2137,9 +1955,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="50" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2149,11 +1964,6 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="32" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -2186,80 +1996,251 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="43" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="32" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="43" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="14" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="14" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3203,16 +3184,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="135"/>
+      <c r="A1" s="73"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="96" t="str">
+      <c r="F1" s="49" t="str">
         <f>Sheet1!E5</f>
         <v>Company Request ID #:*</v>
       </c>
-      <c r="G1" s="97">
+      <c r="G1" s="50">
         <f>Sheet1!F5</f>
         <v>0</v>
       </c>
@@ -3228,137 +3209,137 @@
       <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" s="6" customFormat="1" ht="46.35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="136"/>
+      <c r="A2" s="74"/>
       <c r="D2" s="7"/>
-      <c r="F2" s="95" t="s">
+      <c r="F2" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="G2" s="98">
+      <c r="G2" s="51">
         <f>Sheet1!D7</f>
         <v>0</v>
       </c>
       <c r="Q2" s="8"/>
     </row>
     <row r="3" spans="1:17" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="136"/>
+      <c r="A3" s="74"/>
       <c r="Q3" s="9"/>
     </row>
     <row r="4" spans="1:17" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="136"/>
+      <c r="A4" s="74"/>
       <c r="Q4" s="9"/>
     </row>
     <row r="5" spans="1:17" s="6" customFormat="1" ht="73.349999999999994" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="136"/>
+      <c r="A5" s="74"/>
       <c r="Q5" s="9"/>
     </row>
     <row r="6" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="136"/>
-      <c r="B6" s="140" t="s">
+      <c r="A6" s="74"/>
+      <c r="B6" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="140"/>
-      <c r="D6" s="140"/>
-      <c r="E6" s="140"/>
-      <c r="F6" s="140"/>
-      <c r="G6" s="140"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
       <c r="Q6" s="9"/>
     </row>
     <row r="7" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="137"/>
-      <c r="B7" s="139" t="s">
+      <c r="A7" s="75"/>
+      <c r="B7" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="139"/>
-      <c r="D7" s="139"/>
-      <c r="E7" s="139"/>
-      <c r="F7" s="139"/>
-      <c r="G7" s="139"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
       <c r="Q7" s="9"/>
     </row>
     <row r="8" spans="1:17" s="6" customFormat="1" ht="32.85" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="136"/>
-      <c r="B8" s="138">
+      <c r="A8" s="74"/>
+      <c r="B8" s="76">
         <f>Sheet1!C8</f>
         <v>0</v>
       </c>
-      <c r="C8" s="138"/>
-      <c r="D8" s="138"/>
-      <c r="E8" s="138"/>
-      <c r="F8" s="138"/>
-      <c r="G8" s="138"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
       <c r="Q8" s="9"/>
     </row>
     <row r="9" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="136"/>
-      <c r="B9" s="141" t="str">
+      <c r="A9" s="74"/>
+      <c r="B9" s="79" t="str">
         <f>CONCATENATE("Purchase Request ID #: ",G1," - ",Sheet1!C8,"Charge Code #: ",Sheet1!F6, " - ",F2," ",G2)</f>
         <v>Purchase Request ID #: 0 - Charge Code #: 19 - Revision #: 0</v>
       </c>
-      <c r="C9" s="141"/>
-      <c r="D9" s="141"/>
-      <c r="E9" s="141"/>
-      <c r="F9" s="141"/>
-      <c r="G9" s="141"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
       <c r="Q9" s="9"/>
     </row>
     <row r="10" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="136"/>
-      <c r="B10" s="141"/>
-      <c r="C10" s="141"/>
-      <c r="D10" s="141"/>
-      <c r="E10" s="141"/>
-      <c r="F10" s="141"/>
-      <c r="G10" s="141"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
       <c r="J10" s="13"/>
       <c r="Q10" s="9"/>
     </row>
     <row r="11" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="136"/>
-      <c r="B11" s="103" t="s">
+      <c r="A11" s="74"/>
+      <c r="B11" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="104"/>
-      <c r="D11" s="104"/>
-      <c r="E11" s="105">
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="54">
         <f>IF(AND(Sheet1!F27=0,Sheet1!E27=0),Sheet1!D27,IF(Sheet1!F27=0,Sheet1!E27-Sheet1!D27,Sheet1!F27-Sheet1!E27))</f>
         <v>0</v>
       </c>
-      <c r="F11" s="106"/>
-      <c r="G11" s="107"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="56"/>
       <c r="Q11" s="9"/>
     </row>
     <row r="12" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="136"/>
-      <c r="B12" s="103" t="s">
+      <c r="A12" s="74"/>
+      <c r="B12" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="104"/>
-      <c r="D12" s="104"/>
-      <c r="E12" s="108">
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="57">
         <f>E11*0.06</f>
         <v>0</v>
       </c>
-      <c r="F12" s="106"/>
-      <c r="G12" s="107"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="56"/>
       <c r="Q12" s="9"/>
     </row>
     <row r="13" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="136"/>
-      <c r="B13" s="103" t="s">
+      <c r="A13" s="74"/>
+      <c r="B13" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="104"/>
-      <c r="D13" s="104"/>
-      <c r="E13" s="108">
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="57">
         <f>E11+E12</f>
         <v>0</v>
       </c>
-      <c r="F13" s="106"/>
-      <c r="G13" s="107"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="56"/>
       <c r="Q13" s="9"/>
     </row>
     <row r="14" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="136"/>
+      <c r="A14" s="74"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="10"/>
@@ -3368,139 +3349,139 @@
       <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="136"/>
+      <c r="A15" s="74"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
       <c r="Q15" s="9"/>
     </row>
     <row r="16" spans="1:17" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A16" s="136"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
+      <c r="A16" s="74"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
       <c r="Q16" s="9"/>
     </row>
     <row r="17" spans="1:17" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A17" s="136"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
+      <c r="A17" s="74"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
       <c r="Q17" s="9"/>
     </row>
     <row r="18" spans="1:17" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A18" s="136"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="62"/>
-      <c r="J18" s="62"/>
+      <c r="A18" s="74"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
       <c r="Q18" s="9"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A19" s="136"/>
+      <c r="A19" s="74"/>
       <c r="Q19" s="9"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A20" s="136"/>
+      <c r="A20" s="74"/>
       <c r="Q20" s="9"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A21" s="136"/>
+      <c r="A21" s="74"/>
       <c r="Q21" s="9"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A22" s="136"/>
+      <c r="A22" s="74"/>
       <c r="Q22" s="9"/>
     </row>
     <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="136"/>
-      <c r="C23" s="94">
+      <c r="A23" s="74"/>
+      <c r="C23" s="47">
         <v>0</v>
       </c>
       <c r="Q23" s="9"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A24" s="136"/>
+      <c r="A24" s="74"/>
       <c r="Q24" s="9"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A25" s="136"/>
+      <c r="A25" s="74"/>
       <c r="Q25" s="9"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A26" s="136"/>
+      <c r="A26" s="74"/>
       <c r="Q26" s="9"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A27" s="136"/>
+      <c r="A27" s="74"/>
       <c r="Q27" s="9"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A28" s="136"/>
+      <c r="A28" s="74"/>
       <c r="Q28" s="9"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A29" s="136"/>
+      <c r="A29" s="74"/>
       <c r="Q29" s="9"/>
     </row>
     <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="136"/>
+      <c r="A30" s="74"/>
       <c r="Q30" s="9"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A31" s="136"/>
+      <c r="A31" s="74"/>
       <c r="Q31" s="9"/>
     </row>
     <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="136"/>
+      <c r="A32" s="74"/>
       <c r="Q32" s="9"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A33" s="136"/>
+      <c r="A33" s="74"/>
       <c r="Q33" s="9"/>
     </row>
     <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="136"/>
+      <c r="A34" s="74"/>
       <c r="Q34" s="9"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A35" s="136"/>
+      <c r="A35" s="74"/>
       <c r="Q35" s="9"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A36" s="136"/>
+      <c r="A36" s="74"/>
       <c r="Q36" s="9"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A37" s="136"/>
+      <c r="A37" s="74"/>
       <c r="Q37" s="9"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A38" s="136"/>
+      <c r="A38" s="74"/>
       <c r="Q38" s="9"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A39" s="136"/>
+      <c r="A39" s="74"/>
       <c r="Q39" s="9"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.45">
@@ -3939,10 +3920,10 @@
       <c r="B142" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E142" s="132" t="s">
+      <c r="E142" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="F142" s="133"/>
+      <c r="F142" s="71"/>
       <c r="G142" s="22"/>
       <c r="H142" s="23">
         <v>1</v>
@@ -3953,15 +3934,15 @@
       <c r="J142" s="23">
         <v>0.9</v>
       </c>
-      <c r="K142" s="134" t="s">
+      <c r="K142" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="L142" s="134"/>
-      <c r="M142" s="134"/>
-      <c r="N142" s="134"/>
-      <c r="O142" s="134"/>
-      <c r="P142" s="134"/>
-      <c r="Q142" s="134"/>
+      <c r="L142" s="72"/>
+      <c r="M142" s="72"/>
+      <c r="N142" s="72"/>
+      <c r="O142" s="72"/>
+      <c r="P142" s="72"/>
+      <c r="Q142" s="72"/>
       <c r="S142" s="5">
         <v>1.7</v>
       </c>
@@ -3976,10 +3957,10 @@
       <c r="B143" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E143" s="132" t="s">
+      <c r="E143" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="F143" s="133"/>
+      <c r="F143" s="71"/>
       <c r="G143" s="22"/>
       <c r="H143" s="23">
         <v>1</v>
@@ -3990,15 +3971,15 @@
       <c r="J143" s="24">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K143" s="134" t="s">
+      <c r="K143" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="L143" s="134"/>
-      <c r="M143" s="134"/>
-      <c r="N143" s="134"/>
-      <c r="O143" s="134"/>
-      <c r="P143" s="134"/>
-      <c r="Q143" s="134"/>
+      <c r="L143" s="72"/>
+      <c r="M143" s="72"/>
+      <c r="N143" s="72"/>
+      <c r="O143" s="72"/>
+      <c r="P143" s="72"/>
+      <c r="Q143" s="72"/>
       <c r="S143" s="5">
         <v>12.1</v>
       </c>
@@ -4013,10 +3994,10 @@
       <c r="B144" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E144" s="132" t="s">
+      <c r="E144" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="F144" s="133"/>
+      <c r="F144" s="71"/>
       <c r="G144" s="22"/>
       <c r="H144" s="23">
         <v>1</v>
@@ -4027,15 +4008,15 @@
       <c r="J144" s="24">
         <v>0.75</v>
       </c>
-      <c r="K144" s="134" t="s">
+      <c r="K144" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="L144" s="134"/>
-      <c r="M144" s="134"/>
-      <c r="N144" s="134"/>
-      <c r="O144" s="134"/>
-      <c r="P144" s="134"/>
-      <c r="Q144" s="134"/>
+      <c r="L144" s="72"/>
+      <c r="M144" s="72"/>
+      <c r="N144" s="72"/>
+      <c r="O144" s="72"/>
+      <c r="P144" s="72"/>
+      <c r="Q144" s="72"/>
       <c r="S144" s="5">
         <v>1.7</v>
       </c>
@@ -4655,7 +4636,7 @@
   <dimension ref="A1:H76"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D5" sqref="C5:F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -4671,753 +4652,754 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="126"/>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
     </row>
     <row r="3" spans="1:7" ht="9.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="126"/>
-      <c r="B3" s="126"/>
-      <c r="C3" s="126"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="126"/>
+      <c r="A3" s="67"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
     </row>
     <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="C4" s="151" t="s">
+      <c r="C4" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="152"/>
-      <c r="E4" s="152"/>
-      <c r="F4" s="153"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="82"/>
     </row>
     <row r="5" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="110"/>
-      <c r="D5" s="117"/>
-      <c r="E5" s="36" t="s">
+      <c r="C5" s="86"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="88" t="s">
         <v>121</v>
       </c>
-      <c r="F5" s="67"/>
+      <c r="F5" s="89"/>
     </row>
     <row r="6" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C6" s="110" t="s">
+      <c r="C6" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="109">
+      <c r="D6" s="90">
         <f ca="1">TODAY()</f>
-        <v>44094</v>
-      </c>
-      <c r="E6" s="36" t="s">
+        <v>44108</v>
+      </c>
+      <c r="E6" s="88" t="s">
         <v>120</v>
       </c>
-      <c r="F6" s="42" t="str">
+      <c r="F6" s="91" t="str">
         <f>IF(F7="S","19",IF(F7="M","18","17"))</f>
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="92" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="118">
+      <c r="D7" s="93">
         <v>0</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="94" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="66" t="s">
+      <c r="F7" s="95" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="160"/>
-      <c r="D8" s="161"/>
-      <c r="E8" s="162"/>
-      <c r="F8" s="163"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="99"/>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.4">
-      <c r="C9" s="37" t="str">
+      <c r="C9" s="100" t="str">
         <f>IF(F7="S","Description of Work to be Performed &amp; Estimated Duration of Work on Site",IF(F7="M","Description of Material to be Purchased &amp; Purpose","Equipment Rental Requirement &amp; Duration on Site"))</f>
         <v>Description of Work to be Performed &amp; Estimated Duration of Work on Site</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="39"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="101"/>
+      <c r="F9" s="102"/>
     </row>
     <row r="10" spans="1:7" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C10" s="154"/>
-      <c r="D10" s="155"/>
-      <c r="E10" s="155"/>
-      <c r="F10" s="156"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="104"/>
+      <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:7" ht="15.4" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C11" s="40" t="str">
+      <c r="C11" s="106" t="str">
         <f>IF(F7="S","Duration of Work on Site:",IF(F7="M","CMOA Required (Yes / CMOA Approved / N/A):","Rental Duration on Site:"))</f>
         <v>Duration of Work on Site:</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="D11" s="107" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="91" t="str">
+      <c r="E11" s="108" t="str">
         <f>IF(F7="S","Rate Sheet Attached",IF(F7="E","Gate Access Arranged?","Warranty Offered?"))</f>
         <v>Rate Sheet Attached</v>
       </c>
-      <c r="F11" s="86" t="s">
+      <c r="F11" s="109" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.4" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="125" t="str">
+      <c r="C12" s="110" t="str">
         <f>IF(F7="M","Verified With Material Coordinators Material Not in Stock (Y/N):",IF(F7="E","Equipment has Been Verified to have Tier 4 Engine","Gate Access Required to Enter / Material Gate Pass Required?"))</f>
         <v>Gate Access Required to Enter / Material Gate Pass Required?</v>
       </c>
-      <c r="D12" s="85" t="s">
+      <c r="D12" s="111" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="91" t="s">
+      <c r="E12" s="108" t="s">
         <v>107</v>
       </c>
-      <c r="F12" s="92" t="s">
+      <c r="F12" s="112" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.4">
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="39"/>
+      <c r="D13" s="101"/>
+      <c r="E13" s="101"/>
+      <c r="F13" s="102"/>
     </row>
     <row r="14" spans="1:7" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C14" s="154"/>
-      <c r="D14" s="155"/>
-      <c r="E14" s="155"/>
-      <c r="F14" s="156"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
+      <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="128"/>
-      <c r="C15" s="131" t="str">
+      <c r="B15" s="69"/>
+      <c r="C15" s="113" t="str">
         <f>CONCATENATE("Total Amount Request for Approval (Revision"," ",D7,")")</f>
         <v>Total Amount Request for Approval (Revision 0)</v>
       </c>
-      <c r="D15" s="130">
+      <c r="D15" s="114">
         <f>'Cover Page'!E11</f>
         <v>0</v>
       </c>
-      <c r="E15" s="129"/>
+      <c r="E15" s="115"/>
+      <c r="F15" s="116"/>
     </row>
     <row r="16" spans="1:7" ht="1.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C16" s="111"/>
-      <c r="D16" s="112"/>
-      <c r="E16" s="112"/>
-      <c r="F16" s="113"/>
+      <c r="C16" s="117"/>
+      <c r="D16" s="118"/>
+      <c r="E16" s="118"/>
+      <c r="F16" s="119"/>
     </row>
     <row r="17" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C17" s="72"/>
-      <c r="D17" s="73" t="s">
+      <c r="C17" s="120"/>
+      <c r="D17" s="121" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="73" t="s">
+      <c r="E17" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="74" t="s">
+      <c r="F17" s="122" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="3:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C18" s="41"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="69"/>
+      <c r="C18" s="123"/>
+      <c r="D18" s="124"/>
+      <c r="E18" s="124"/>
+      <c r="F18" s="125"/>
     </row>
     <row r="19" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C19" s="41" t="str">
+      <c r="C19" s="123" t="str">
         <f>IF(D5&gt;0,"Subtotal Price:*","Estimated Subtotal Price:*")</f>
         <v>Estimated Subtotal Price:*</v>
       </c>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="69"/>
+      <c r="D19" s="124"/>
+      <c r="E19" s="124"/>
+      <c r="F19" s="125"/>
     </row>
     <row r="20" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C20" s="41" t="str">
+      <c r="C20" s="123" t="str">
         <f>IF($F$7="S","PST Cost (if excluded supplier from quote):",IF($F$7="M","Additional Warranty Cost (If applicable):","Rental Protection Insurance Cost:"))</f>
         <v>PST Cost (if excluded supplier from quote):</v>
       </c>
-      <c r="D20" s="68">
+      <c r="D20" s="124">
         <v>0</v>
       </c>
-      <c r="E20" s="68">
+      <c r="E20" s="124">
         <v>0</v>
       </c>
-      <c r="F20" s="69">
+      <c r="F20" s="125">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C21" s="41" t="str">
+      <c r="C21" s="123" t="str">
         <f>IF(OR($F$7="E",$F$7="S"),"Mobilization / Demob Cost (if excluded supplier from quote):","Freight (if excluded supplier from quote):")</f>
         <v>Mobilization / Demob Cost (if excluded supplier from quote):</v>
       </c>
-      <c r="D21" s="68">
+      <c r="D21" s="124">
         <v>0</v>
       </c>
-      <c r="E21" s="68">
+      <c r="E21" s="124">
         <v>0</v>
       </c>
-      <c r="F21" s="69">
+      <c r="F21" s="125">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C22" s="41" t="str">
+      <c r="C22" s="123" t="str">
         <f>IF($F$7="S","Site Orientation Cost (if excluded supplier from quote):",IF($F$7="M","Environmental Fees (if excluded supplier from quote):","Equipment Disinfection Cost if Out of Province Rental:"))</f>
         <v>Site Orientation Cost (if excluded supplier from quote):</v>
       </c>
-      <c r="D22" s="68">
+      <c r="D22" s="124">
         <v>0</v>
       </c>
-      <c r="E22" s="68">
+      <c r="E22" s="124">
         <v>0</v>
       </c>
-      <c r="F22" s="69">
+      <c r="F22" s="125">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="3:6" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C23" s="43" t="s">
+      <c r="C23" s="126" t="s">
         <v>100</v>
       </c>
-      <c r="D23" s="70">
+      <c r="D23" s="127">
         <v>0</v>
       </c>
-      <c r="E23" s="70">
+      <c r="E23" s="127">
         <v>0</v>
       </c>
-      <c r="F23" s="71">
+      <c r="F23" s="128">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="87">
+      <c r="D24" s="129">
         <f>SUM(D19:D23)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="87">
+      <c r="E24" s="129">
         <f>SUM(E19:E23)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="88">
+      <c r="F24" s="130">
         <f>SUM(F19:F23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C25" s="41" t="s">
+      <c r="C25" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="89">
+      <c r="D25" s="131">
         <v>0</v>
       </c>
-      <c r="E25" s="89">
+      <c r="E25" s="131">
         <v>0</v>
       </c>
-      <c r="F25" s="90">
+      <c r="F25" s="132">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="3:6" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C26" s="43" t="s">
+      <c r="C26" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D26" s="133">
         <f>D24*D25</f>
         <v>0</v>
       </c>
-      <c r="E26" s="34">
+      <c r="E26" s="133">
         <f>E24*E25</f>
         <v>0</v>
       </c>
-      <c r="F26" s="49">
+      <c r="F26" s="134">
         <f>F24*F25</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="3:6" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C27" s="52" t="s">
+      <c r="C27" s="135" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="53">
+      <c r="D27" s="136">
         <f>D26+D24</f>
         <v>0</v>
       </c>
-      <c r="E27" s="53">
+      <c r="E27" s="136">
         <f>E26+E24</f>
         <v>0</v>
       </c>
-      <c r="F27" s="54">
+      <c r="F27" s="137">
         <f>F26+F24</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="3:6" ht="1.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="111"/>
-      <c r="D28" s="112"/>
-      <c r="E28" s="112"/>
-      <c r="F28" s="113"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="118"/>
+      <c r="E28" s="118"/>
+      <c r="F28" s="119"/>
     </row>
     <row r="29" spans="3:6" ht="22.15" x14ac:dyDescent="0.4">
-      <c r="C29" s="51" t="s">
+      <c r="C29" s="138" t="s">
         <v>116</v>
       </c>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="50"/>
+      <c r="D29" s="139"/>
+      <c r="E29" s="139"/>
+      <c r="F29" s="140"/>
     </row>
     <row r="30" spans="3:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="157"/>
-      <c r="D30" s="158"/>
-      <c r="E30" s="158"/>
-      <c r="F30" s="159"/>
+      <c r="C30" s="141"/>
+      <c r="D30" s="142"/>
+      <c r="E30" s="142"/>
+      <c r="F30" s="143"/>
     </row>
     <row r="31" spans="3:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C31" s="51" t="s">
+      <c r="C31" s="138" t="s">
         <v>117</v>
       </c>
-      <c r="D31" s="145"/>
-      <c r="E31" s="145"/>
-      <c r="F31" s="146"/>
+      <c r="D31" s="144"/>
+      <c r="E31" s="144"/>
+      <c r="F31" s="145"/>
     </row>
     <row r="32" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C32" s="99" t="s">
+      <c r="C32" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="100">
+      <c r="D32" s="147">
         <f>D27</f>
         <v>0</v>
       </c>
-      <c r="E32" s="101">
+      <c r="E32" s="147">
         <f>E27</f>
         <v>0</v>
       </c>
-      <c r="F32" s="102">
+      <c r="F32" s="148">
         <f>F27</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C33" s="75" t="s">
+      <c r="C33" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="56" t="s">
+      <c r="D33" s="150" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="56" t="s">
+      <c r="E33" s="150" t="s">
         <v>66</v>
       </c>
-      <c r="F33" s="77" t="s">
+      <c r="F33" s="151" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="34" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="149" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="56" t="s">
+      <c r="D34" s="150" t="s">
         <v>64</v>
       </c>
-      <c r="E34" s="56" t="s">
+      <c r="E34" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="F34" s="77" t="s">
+      <c r="F34" s="151" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="35" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C35" s="75" t="s">
+      <c r="C35" s="149" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="56" t="s">
+      <c r="D35" s="150" t="s">
         <v>63</v>
       </c>
-      <c r="E35" s="56" t="s">
+      <c r="E35" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="77" t="s">
+      <c r="F35" s="151" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="36" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C36" s="75" t="s">
+      <c r="C36" s="149" t="s">
         <v>102</v>
       </c>
-      <c r="D36" s="56" t="s">
+      <c r="D36" s="150" t="s">
         <v>63</v>
       </c>
-      <c r="E36" s="56" t="s">
+      <c r="E36" s="150" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="77" t="s">
+      <c r="F36" s="151" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="37" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C37" s="75" t="s">
+      <c r="C37" s="149" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="56" t="s">
+      <c r="D37" s="150" t="s">
         <v>64</v>
       </c>
-      <c r="E37" s="56"/>
-      <c r="F37" s="77"/>
+      <c r="E37" s="150"/>
+      <c r="F37" s="151"/>
     </row>
     <row r="38" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C38" s="41" t="s">
+      <c r="C38" s="123" t="s">
         <v>111</v>
       </c>
-      <c r="D38" s="93"/>
-      <c r="E38" s="149"/>
-      <c r="F38" s="150"/>
+      <c r="D38" s="152"/>
+      <c r="E38" s="153"/>
+      <c r="F38" s="145"/>
     </row>
     <row r="39" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C39" s="41" t="s">
+      <c r="C39" s="123" t="s">
         <v>108</v>
       </c>
-      <c r="D39" s="35" t="s">
+      <c r="D39" s="139" t="s">
         <v>110</v>
       </c>
-      <c r="E39" s="35"/>
-      <c r="F39" s="50"/>
+      <c r="E39" s="139"/>
+      <c r="F39" s="140"/>
     </row>
     <row r="40" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C40" s="41"/>
-      <c r="D40" s="35" t="s">
+      <c r="C40" s="123"/>
+      <c r="D40" s="139" t="s">
         <v>109</v>
       </c>
-      <c r="E40" s="35"/>
-      <c r="F40" s="50"/>
+      <c r="E40" s="139"/>
+      <c r="F40" s="140"/>
     </row>
     <row r="41" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C41" s="41"/>
-      <c r="D41" s="35" t="s">
+      <c r="C41" s="123"/>
+      <c r="D41" s="139" t="s">
         <v>122</v>
       </c>
-      <c r="E41" s="35"/>
-      <c r="F41" s="50"/>
+      <c r="E41" s="139"/>
+      <c r="F41" s="140"/>
     </row>
     <row r="42" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C42" s="41"/>
-      <c r="D42" s="35" t="s">
+      <c r="C42" s="123"/>
+      <c r="D42" s="139" t="s">
         <v>112</v>
       </c>
-      <c r="E42" s="35"/>
-      <c r="F42" s="50"/>
+      <c r="E42" s="139"/>
+      <c r="F42" s="140"/>
     </row>
     <row r="43" spans="3:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C43" s="55" t="s">
+      <c r="C43" s="92" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="147"/>
-      <c r="E43" s="147"/>
-      <c r="F43" s="148"/>
+      <c r="D43" s="154"/>
+      <c r="E43" s="154"/>
+      <c r="F43" s="155"/>
     </row>
     <row r="44" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C44" s="75" t="s">
+      <c r="C44" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="76">
+      <c r="D44" s="124">
         <v>0</v>
       </c>
-      <c r="E44" s="68"/>
-      <c r="F44" s="69"/>
+      <c r="E44" s="124"/>
+      <c r="F44" s="125"/>
     </row>
     <row r="45" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C45" s="75" t="s">
+      <c r="C45" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="56" t="s">
+      <c r="D45" s="150" t="s">
         <v>65</v>
       </c>
-      <c r="E45" s="56" t="s">
+      <c r="E45" s="150" t="s">
         <v>66</v>
       </c>
-      <c r="F45" s="77" t="s">
+      <c r="F45" s="151" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="46" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C46" s="75" t="s">
+      <c r="C46" s="149" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="56" t="s">
+      <c r="D46" s="150" t="s">
         <v>65</v>
       </c>
-      <c r="E46" s="56" t="s">
+      <c r="E46" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="F46" s="77" t="s">
+      <c r="F46" s="151" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="47" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C47" s="75" t="s">
+      <c r="C47" s="149" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="56" t="s">
+      <c r="D47" s="150" t="s">
         <v>65</v>
       </c>
-      <c r="E47" s="56" t="s">
+      <c r="E47" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="77" t="s">
+      <c r="F47" s="151" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="48" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C48" s="75" t="s">
+      <c r="C48" s="149" t="s">
         <v>102</v>
       </c>
-      <c r="D48" s="56" t="s">
+      <c r="D48" s="150" t="s">
         <v>65</v>
       </c>
-      <c r="E48" s="56" t="s">
+      <c r="E48" s="150" t="s">
         <v>13</v>
       </c>
-      <c r="F48" s="77" t="s">
+      <c r="F48" s="151" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="49" spans="3:8" ht="15" x14ac:dyDescent="0.35">
-      <c r="C49" s="75" t="s">
+      <c r="C49" s="149" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="56" t="s">
+      <c r="D49" s="150" t="s">
         <v>65</v>
       </c>
-      <c r="E49" s="56"/>
-      <c r="F49" s="77"/>
+      <c r="E49" s="150"/>
+      <c r="F49" s="151"/>
     </row>
     <row r="50" spans="3:8" ht="1.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C50" s="111"/>
-      <c r="D50" s="112"/>
-      <c r="E50" s="112"/>
-      <c r="F50" s="113"/>
+      <c r="C50" s="117"/>
+      <c r="D50" s="118"/>
+      <c r="E50" s="118"/>
+      <c r="F50" s="119"/>
     </row>
     <row r="51" spans="3:8" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C51" s="55" t="s">
+      <c r="C51" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="D51" s="147"/>
-      <c r="E51" s="147"/>
-      <c r="F51" s="148"/>
+      <c r="D51" s="154"/>
+      <c r="E51" s="154"/>
+      <c r="F51" s="155"/>
     </row>
     <row r="52" spans="3:8" ht="15" x14ac:dyDescent="0.35">
-      <c r="C52" s="75" t="s">
+      <c r="C52" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="D52" s="76">
+      <c r="D52" s="124">
         <v>0</v>
       </c>
-      <c r="E52" s="68"/>
-      <c r="F52" s="69"/>
+      <c r="E52" s="124"/>
+      <c r="F52" s="125"/>
     </row>
     <row r="53" spans="3:8" ht="15" x14ac:dyDescent="0.35">
-      <c r="C53" s="75" t="s">
+      <c r="C53" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="56" t="s">
+      <c r="D53" s="150" t="s">
         <v>65</v>
       </c>
-      <c r="E53" s="56" t="s">
+      <c r="E53" s="150" t="s">
         <v>66</v>
       </c>
-      <c r="F53" s="77" t="s">
+      <c r="F53" s="151" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="54" spans="3:8" ht="15" x14ac:dyDescent="0.35">
-      <c r="C54" s="75" t="s">
+      <c r="C54" s="149" t="s">
         <v>5</v>
       </c>
-      <c r="D54" s="56" t="s">
+      <c r="D54" s="150" t="s">
         <v>65</v>
       </c>
-      <c r="E54" s="56" t="s">
+      <c r="E54" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="F54" s="77" t="s">
+      <c r="F54" s="151" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="55" spans="3:8" ht="15" x14ac:dyDescent="0.35">
-      <c r="C55" s="75" t="s">
+      <c r="C55" s="149" t="s">
         <v>6</v>
       </c>
-      <c r="D55" s="56" t="s">
+      <c r="D55" s="150" t="s">
         <v>65</v>
       </c>
-      <c r="E55" s="56" t="s">
+      <c r="E55" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="F55" s="77" t="s">
+      <c r="F55" s="151" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="56" spans="3:8" ht="15" x14ac:dyDescent="0.35">
-      <c r="C56" s="75" t="s">
+      <c r="C56" s="149" t="s">
         <v>102</v>
       </c>
-      <c r="D56" s="56" t="s">
+      <c r="D56" s="150" t="s">
         <v>65</v>
       </c>
-      <c r="E56" s="56" t="s">
+      <c r="E56" s="150" t="s">
         <v>13</v>
       </c>
-      <c r="F56" s="77" t="s">
+      <c r="F56" s="151" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="57" spans="3:8" ht="15.4" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C57" s="78" t="s">
+      <c r="C57" s="156" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="79" t="s">
+      <c r="D57" s="157" t="s">
         <v>65</v>
       </c>
-      <c r="E57" s="79"/>
-      <c r="F57" s="80"/>
+      <c r="E57" s="157"/>
+      <c r="F57" s="158"/>
     </row>
     <row r="58" spans="3:8" ht="1.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C58" s="111"/>
-      <c r="D58" s="112"/>
-      <c r="E58" s="112"/>
-      <c r="F58" s="113"/>
+      <c r="C58" s="117"/>
+      <c r="D58" s="118"/>
+      <c r="E58" s="118"/>
+      <c r="F58" s="119"/>
     </row>
     <row r="59" spans="3:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C59" s="48" t="s">
+      <c r="C59" s="120" t="s">
         <v>67</v>
       </c>
-      <c r="D59" s="81"/>
-      <c r="E59" s="81"/>
-      <c r="F59" s="82"/>
+      <c r="D59" s="159"/>
+      <c r="E59" s="159"/>
+      <c r="F59" s="160"/>
     </row>
     <row r="60" spans="3:8" ht="15" x14ac:dyDescent="0.4">
-      <c r="C60" s="41" t="s">
+      <c r="C60" s="123" t="s">
         <v>68</v>
       </c>
-      <c r="D60" s="56"/>
-      <c r="E60" s="56" t="s">
+      <c r="D60" s="150"/>
+      <c r="E60" s="150" t="s">
         <v>101</v>
       </c>
-      <c r="F60" s="83">
+      <c r="F60" s="161">
         <f ca="1">TODAY()</f>
-        <v>44094</v>
+        <v>44108</v>
       </c>
     </row>
     <row r="61" spans="3:8" ht="15" x14ac:dyDescent="0.4">
-      <c r="C61" s="41" t="s">
+      <c r="C61" s="123" t="s">
         <v>69</v>
       </c>
-      <c r="D61" s="56"/>
-      <c r="E61" s="56" t="s">
+      <c r="D61" s="150"/>
+      <c r="E61" s="150" t="s">
         <v>101</v>
       </c>
-      <c r="F61" s="83"/>
+      <c r="F61" s="161"/>
     </row>
     <row r="62" spans="3:8" ht="15.4" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C62" s="116"/>
-      <c r="D62" s="119" t="s">
+      <c r="C62" s="60"/>
+      <c r="D62" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="E62" s="120" t="s">
+      <c r="E62" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="F62" s="121" t="s">
+      <c r="F62" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="G62" s="45"/>
-      <c r="H62" s="45"/>
+      <c r="G62" s="34"/>
+      <c r="H62" s="34"/>
     </row>
     <row r="63" spans="3:8" ht="23" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C63" s="122" t="s">
+      <c r="C63" s="64" t="s">
         <v>123</v>
       </c>
-      <c r="D63" s="127"/>
-      <c r="E63" s="81"/>
-      <c r="F63" s="124"/>
-      <c r="G63" s="46"/>
-      <c r="H63" s="46"/>
+      <c r="D63" s="68"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="66"/>
+      <c r="G63" s="35"/>
+      <c r="H63" s="35"/>
     </row>
     <row r="64" spans="3:8" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C64" s="115" t="s">
+      <c r="C64" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="D64" s="142"/>
-      <c r="E64" s="143"/>
-      <c r="F64" s="144"/>
+      <c r="D64" s="83"/>
+      <c r="E64" s="84"/>
+      <c r="F64" s="85"/>
     </row>
     <row r="65" spans="1:8" ht="23" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="47">
+      <c r="A65" s="36">
         <v>10000</v>
       </c>
-      <c r="B65" s="47"/>
-      <c r="C65" s="123" t="str">
+      <c r="B65" s="36"/>
+      <c r="C65" s="65" t="str">
         <f>IF(OR($D$27&gt;$A$65,$E$27&gt;$A$65,$F$27&gt;$A$65),"Client Maury Simoneau (Up to $50,000.00)"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D65" s="127"/>
-      <c r="E65" s="81"/>
-      <c r="F65" s="124"/>
-      <c r="G65" s="46"/>
-      <c r="H65" s="46"/>
+      <c r="D65" s="68"/>
+      <c r="E65" s="46"/>
+      <c r="F65" s="66"/>
+      <c r="G65" s="35"/>
+      <c r="H65" s="35"/>
     </row>
     <row r="66" spans="1:8" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C66" s="114" t="str">
+      <c r="C66" s="58" t="str">
         <f>IF(OR($D$27&gt;$A$65,$E$27&gt;$A$65,$F$27&gt;$A$65),"Comment from Maury Simoneau (If Applicable):"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D66" s="142"/>
-      <c r="E66" s="143"/>
-      <c r="F66" s="144"/>
+      <c r="D66" s="83"/>
+      <c r="E66" s="84"/>
+      <c r="F66" s="85"/>
     </row>
     <row r="67" spans="1:8" ht="23" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="47">
+      <c r="A67" s="36">
         <v>50000</v>
       </c>
-      <c r="B67" s="47"/>
-      <c r="C67" s="123" t="str">
+      <c r="B67" s="36"/>
+      <c r="C67" s="65" t="str">
         <f>IF(OR($D$27&gt;$A$67,$E$27&gt;$A$67,$F$27&gt;$A$67),"Client Chris Whorton (+$50,000.00)"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D67" s="127"/>
-      <c r="E67" s="81"/>
-      <c r="F67" s="124"/>
-      <c r="G67" s="46"/>
-      <c r="H67" s="46"/>
+      <c r="D67" s="68"/>
+      <c r="E67" s="46"/>
+      <c r="F67" s="66"/>
+      <c r="G67" s="35"/>
+      <c r="H67" s="35"/>
     </row>
     <row r="68" spans="1:8" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C68" s="115" t="str">
+      <c r="C68" s="59" t="str">
         <f>IF(OR($D$27&gt;$A$67,$E$27&gt;$A$67,$F$27&gt;$A$67),"Comment from Chris Whorton (If Applicable):"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D68" s="142"/>
-      <c r="E68" s="143"/>
-      <c r="F68" s="144"/>
+      <c r="D68" s="83"/>
+      <c r="E68" s="84"/>
+      <c r="F68" s="85"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C69" s="33"/>
@@ -5469,11 +5451,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C8:F8"/>
     <mergeCell ref="D64:F64"/>
     <mergeCell ref="D66:F66"/>
     <mergeCell ref="D68:F68"/>
@@ -5481,6 +5458,11 @@
     <mergeCell ref="D43:F43"/>
     <mergeCell ref="D51:F51"/>
     <mergeCell ref="E38:F38"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C8:F8"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Arranged with Same Error Opening
</commit_message>
<xml_diff>
--- a/PurchaseRequestApproval/wwwroot/files/tmp/pratmp_3.xlsx
+++ b/PurchaseRequestApproval/wwwroot/files/tmp/pratmp_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ME\C#\Projects\PurchaseRequestApproval\PurchaseRequestApproval\wwwroot\files\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B2BB9E-1EA1-4F90-B49C-CB9093B99C7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422542FD-8762-41F3-A56B-6BB831B87516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1122,7 +1122,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1137,7 +1137,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1793,7 +1805,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1861,6 +1873,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1868,6 +1901,22 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1893,10 +1942,103 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="169" fontId="14" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="14" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1910,6 +2052,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="3" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="3" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1928,22 +2086,46 @@
     <xf numFmtId="165" fontId="11" fillId="0" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1955,6 +2137,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="50" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1964,6 +2149,11 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="32" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1996,6 +2186,36 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="43" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2005,242 +2225,41 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="32" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="43" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3184,16 +3203,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="73"/>
+      <c r="A1" s="135"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="49" t="str">
+      <c r="F1" s="96" t="str">
         <f>Sheet1!E5</f>
         <v>Company Request ID #:*</v>
       </c>
-      <c r="G1" s="50">
+      <c r="G1" s="97">
         <f>Sheet1!F5</f>
         <v>0</v>
       </c>
@@ -3209,137 +3228,137 @@
       <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" s="6" customFormat="1" ht="46.35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="74"/>
+      <c r="A2" s="136"/>
       <c r="D2" s="7"/>
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="95" t="s">
         <v>113</v>
       </c>
-      <c r="G2" s="51">
+      <c r="G2" s="98">
         <f>Sheet1!D7</f>
         <v>0</v>
       </c>
       <c r="Q2" s="8"/>
     </row>
     <row r="3" spans="1:17" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="74"/>
+      <c r="A3" s="136"/>
       <c r="Q3" s="9"/>
     </row>
     <row r="4" spans="1:17" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="74"/>
+      <c r="A4" s="136"/>
       <c r="Q4" s="9"/>
     </row>
     <row r="5" spans="1:17" s="6" customFormat="1" ht="73.349999999999994" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="74"/>
+      <c r="A5" s="136"/>
       <c r="Q5" s="9"/>
     </row>
     <row r="6" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="74"/>
-      <c r="B6" s="78" t="s">
+      <c r="A6" s="136"/>
+      <c r="B6" s="140" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
+      <c r="F6" s="140"/>
+      <c r="G6" s="140"/>
       <c r="Q6" s="9"/>
     </row>
     <row r="7" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="75"/>
-      <c r="B7" s="77" t="s">
+      <c r="A7" s="137"/>
+      <c r="B7" s="139" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
       <c r="Q7" s="9"/>
     </row>
     <row r="8" spans="1:17" s="6" customFormat="1" ht="32.85" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="74"/>
-      <c r="B8" s="76">
+      <c r="A8" s="136"/>
+      <c r="B8" s="138">
         <f>Sheet1!C8</f>
         <v>0</v>
       </c>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
+      <c r="C8" s="138"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="138"/>
+      <c r="F8" s="138"/>
+      <c r="G8" s="138"/>
       <c r="Q8" s="9"/>
     </row>
     <row r="9" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="74"/>
-      <c r="B9" s="79" t="str">
+      <c r="A9" s="136"/>
+      <c r="B9" s="141" t="str">
         <f>CONCATENATE("Purchase Request ID #: ",G1," - ",Sheet1!C8,"Charge Code #: ",Sheet1!F6, " - ",F2," ",G2)</f>
         <v>Purchase Request ID #: 0 - Charge Code #: 19 - Revision #: 0</v>
       </c>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="G9" s="79"/>
+      <c r="C9" s="141"/>
+      <c r="D9" s="141"/>
+      <c r="E9" s="141"/>
+      <c r="F9" s="141"/>
+      <c r="G9" s="141"/>
       <c r="Q9" s="9"/>
     </row>
     <row r="10" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="74"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
+      <c r="A10" s="136"/>
+      <c r="B10" s="141"/>
+      <c r="C10" s="141"/>
+      <c r="D10" s="141"/>
+      <c r="E10" s="141"/>
+      <c r="F10" s="141"/>
+      <c r="G10" s="141"/>
       <c r="J10" s="13"/>
       <c r="Q10" s="9"/>
     </row>
     <row r="11" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="74"/>
-      <c r="B11" s="52" t="s">
+      <c r="A11" s="136"/>
+      <c r="B11" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="54">
+      <c r="C11" s="104"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="105">
         <f>IF(AND(Sheet1!F27=0,Sheet1!E27=0),Sheet1!D27,IF(Sheet1!F27=0,Sheet1!E27-Sheet1!D27,Sheet1!F27-Sheet1!E27))</f>
         <v>0</v>
       </c>
-      <c r="F11" s="55"/>
-      <c r="G11" s="56"/>
+      <c r="F11" s="106"/>
+      <c r="G11" s="107"/>
       <c r="Q11" s="9"/>
     </row>
     <row r="12" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="74"/>
-      <c r="B12" s="52" t="s">
+      <c r="A12" s="136"/>
+      <c r="B12" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="57">
+      <c r="C12" s="104"/>
+      <c r="D12" s="104"/>
+      <c r="E12" s="108">
         <f>E11*0.06</f>
         <v>0</v>
       </c>
-      <c r="F12" s="55"/>
-      <c r="G12" s="56"/>
+      <c r="F12" s="106"/>
+      <c r="G12" s="107"/>
       <c r="Q12" s="9"/>
     </row>
     <row r="13" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="74"/>
-      <c r="B13" s="52" t="s">
+      <c r="A13" s="136"/>
+      <c r="B13" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="57">
+      <c r="C13" s="104"/>
+      <c r="D13" s="104"/>
+      <c r="E13" s="108">
         <f>E11+E12</f>
         <v>0</v>
       </c>
-      <c r="F13" s="55"/>
-      <c r="G13" s="56"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="107"/>
       <c r="Q13" s="9"/>
     </row>
     <row r="14" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="74"/>
+      <c r="A14" s="136"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="10"/>
@@ -3349,139 +3368,139 @@
       <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="1:17" s="6" customFormat="1" ht="32.85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="74"/>
+      <c r="A15" s="136"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
       <c r="Q15" s="9"/>
     </row>
     <row r="16" spans="1:17" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A16" s="74"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="A16" s="136"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="62"/>
       <c r="Q16" s="9"/>
     </row>
     <row r="17" spans="1:17" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A17" s="74"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="A17" s="136"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
       <c r="Q17" s="9"/>
     </row>
     <row r="18" spans="1:17" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A18" s="74"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="A18" s="136"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="62"/>
+      <c r="J18" s="62"/>
       <c r="Q18" s="9"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A19" s="74"/>
+      <c r="A19" s="136"/>
       <c r="Q19" s="9"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A20" s="74"/>
+      <c r="A20" s="136"/>
       <c r="Q20" s="9"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A21" s="74"/>
+      <c r="A21" s="136"/>
       <c r="Q21" s="9"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A22" s="74"/>
+      <c r="A22" s="136"/>
       <c r="Q22" s="9"/>
     </row>
     <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="74"/>
-      <c r="C23" s="47">
+      <c r="A23" s="136"/>
+      <c r="C23" s="94">
         <v>0</v>
       </c>
       <c r="Q23" s="9"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A24" s="74"/>
+      <c r="A24" s="136"/>
       <c r="Q24" s="9"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A25" s="74"/>
+      <c r="A25" s="136"/>
       <c r="Q25" s="9"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A26" s="74"/>
+      <c r="A26" s="136"/>
       <c r="Q26" s="9"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A27" s="74"/>
+      <c r="A27" s="136"/>
       <c r="Q27" s="9"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A28" s="74"/>
+      <c r="A28" s="136"/>
       <c r="Q28" s="9"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A29" s="74"/>
+      <c r="A29" s="136"/>
       <c r="Q29" s="9"/>
     </row>
     <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="74"/>
+      <c r="A30" s="136"/>
       <c r="Q30" s="9"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A31" s="74"/>
+      <c r="A31" s="136"/>
       <c r="Q31" s="9"/>
     </row>
     <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="74"/>
+      <c r="A32" s="136"/>
       <c r="Q32" s="9"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A33" s="74"/>
+      <c r="A33" s="136"/>
       <c r="Q33" s="9"/>
     </row>
     <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="74"/>
+      <c r="A34" s="136"/>
       <c r="Q34" s="9"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A35" s="74"/>
+      <c r="A35" s="136"/>
       <c r="Q35" s="9"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A36" s="74"/>
+      <c r="A36" s="136"/>
       <c r="Q36" s="9"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A37" s="74"/>
+      <c r="A37" s="136"/>
       <c r="Q37" s="9"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A38" s="74"/>
+      <c r="A38" s="136"/>
       <c r="Q38" s="9"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A39" s="74"/>
+      <c r="A39" s="136"/>
       <c r="Q39" s="9"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.45">
@@ -3920,10 +3939,10 @@
       <c r="B142" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E142" s="70" t="s">
+      <c r="E142" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="F142" s="71"/>
+      <c r="F142" s="133"/>
       <c r="G142" s="22"/>
       <c r="H142" s="23">
         <v>1</v>
@@ -3934,15 +3953,15 @@
       <c r="J142" s="23">
         <v>0.9</v>
       </c>
-      <c r="K142" s="72" t="s">
+      <c r="K142" s="134" t="s">
         <v>21</v>
       </c>
-      <c r="L142" s="72"/>
-      <c r="M142" s="72"/>
-      <c r="N142" s="72"/>
-      <c r="O142" s="72"/>
-      <c r="P142" s="72"/>
-      <c r="Q142" s="72"/>
+      <c r="L142" s="134"/>
+      <c r="M142" s="134"/>
+      <c r="N142" s="134"/>
+      <c r="O142" s="134"/>
+      <c r="P142" s="134"/>
+      <c r="Q142" s="134"/>
       <c r="S142" s="5">
         <v>1.7</v>
       </c>
@@ -3957,10 +3976,10 @@
       <c r="B143" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E143" s="70" t="s">
+      <c r="E143" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="F143" s="71"/>
+      <c r="F143" s="133"/>
       <c r="G143" s="22"/>
       <c r="H143" s="23">
         <v>1</v>
@@ -3971,15 +3990,15 @@
       <c r="J143" s="24">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K143" s="72" t="s">
+      <c r="K143" s="134" t="s">
         <v>24</v>
       </c>
-      <c r="L143" s="72"/>
-      <c r="M143" s="72"/>
-      <c r="N143" s="72"/>
-      <c r="O143" s="72"/>
-      <c r="P143" s="72"/>
-      <c r="Q143" s="72"/>
+      <c r="L143" s="134"/>
+      <c r="M143" s="134"/>
+      <c r="N143" s="134"/>
+      <c r="O143" s="134"/>
+      <c r="P143" s="134"/>
+      <c r="Q143" s="134"/>
       <c r="S143" s="5">
         <v>12.1</v>
       </c>
@@ -3994,10 +4013,10 @@
       <c r="B144" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E144" s="70" t="s">
+      <c r="E144" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="F144" s="71"/>
+      <c r="F144" s="133"/>
       <c r="G144" s="22"/>
       <c r="H144" s="23">
         <v>1</v>
@@ -4008,15 +4027,15 @@
       <c r="J144" s="24">
         <v>0.75</v>
       </c>
-      <c r="K144" s="72" t="s">
+      <c r="K144" s="134" t="s">
         <v>26</v>
       </c>
-      <c r="L144" s="72"/>
-      <c r="M144" s="72"/>
-      <c r="N144" s="72"/>
-      <c r="O144" s="72"/>
-      <c r="P144" s="72"/>
-      <c r="Q144" s="72"/>
+      <c r="L144" s="134"/>
+      <c r="M144" s="134"/>
+      <c r="N144" s="134"/>
+      <c r="O144" s="134"/>
+      <c r="P144" s="134"/>
+      <c r="Q144" s="134"/>
       <c r="S144" s="5">
         <v>1.7</v>
       </c>
@@ -4636,7 +4655,7 @@
   <dimension ref="A1:H76"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="C5:F61"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -4652,754 +4671,753 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="67"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
+      <c r="A2" s="126"/>
+      <c r="B2" s="126"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
     </row>
     <row r="3" spans="1:7" ht="9.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="67"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
+      <c r="A3" s="126"/>
+      <c r="B3" s="126"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
     </row>
     <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="151" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="82"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="153"/>
     </row>
     <row r="5" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="86"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="88" t="s">
+      <c r="C5" s="110"/>
+      <c r="D5" s="117"/>
+      <c r="E5" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="F5" s="89"/>
+      <c r="F5" s="67"/>
     </row>
     <row r="6" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C6" s="86" t="s">
+      <c r="C6" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="90">
+      <c r="D6" s="109">
         <f ca="1">TODAY()</f>
-        <v>44108</v>
-      </c>
-      <c r="E6" s="88" t="s">
+        <v>44094</v>
+      </c>
+      <c r="E6" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="F6" s="91" t="str">
+      <c r="F6" s="42" t="str">
         <f>IF(F7="S","19",IF(F7="M","18","17"))</f>
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C7" s="92" t="s">
+      <c r="C7" s="55" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="93">
+      <c r="D7" s="118">
         <v>0</v>
       </c>
-      <c r="E7" s="94" t="s">
+      <c r="E7" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="95" t="s">
+      <c r="F7" s="66" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="96"/>
-      <c r="D8" s="97"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="99"/>
+      <c r="C8" s="160"/>
+      <c r="D8" s="161"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="163"/>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.4">
-      <c r="C9" s="100" t="str">
+      <c r="C9" s="37" t="str">
         <f>IF(F7="S","Description of Work to be Performed &amp; Estimated Duration of Work on Site",IF(F7="M","Description of Material to be Purchased &amp; Purpose","Equipment Rental Requirement &amp; Duration on Site"))</f>
         <v>Description of Work to be Performed &amp; Estimated Duration of Work on Site</v>
       </c>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="102"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="39"/>
     </row>
     <row r="10" spans="1:7" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C10" s="103"/>
-      <c r="D10" s="104"/>
-      <c r="E10" s="104"/>
-      <c r="F10" s="105"/>
+      <c r="C10" s="154"/>
+      <c r="D10" s="155"/>
+      <c r="E10" s="155"/>
+      <c r="F10" s="156"/>
     </row>
     <row r="11" spans="1:7" ht="15.4" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C11" s="106" t="str">
+      <c r="C11" s="40" t="str">
         <f>IF(F7="S","Duration of Work on Site:",IF(F7="M","CMOA Required (Yes / CMOA Approved / N/A):","Rental Duration on Site:"))</f>
         <v>Duration of Work on Site:</v>
       </c>
-      <c r="D11" s="107" t="s">
+      <c r="D11" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="108" t="str">
+      <c r="E11" s="91" t="str">
         <f>IF(F7="S","Rate Sheet Attached",IF(F7="E","Gate Access Arranged?","Warranty Offered?"))</f>
         <v>Rate Sheet Attached</v>
       </c>
-      <c r="F11" s="109" t="s">
+      <c r="F11" s="86" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.4" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="110" t="str">
+      <c r="C12" s="125" t="str">
         <f>IF(F7="M","Verified With Material Coordinators Material Not in Stock (Y/N):",IF(F7="E","Equipment has Been Verified to have Tier 4 Engine","Gate Access Required to Enter / Material Gate Pass Required?"))</f>
         <v>Gate Access Required to Enter / Material Gate Pass Required?</v>
       </c>
-      <c r="D12" s="111" t="s">
+      <c r="D12" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="108" t="s">
+      <c r="E12" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="F12" s="112" t="s">
+      <c r="F12" s="92" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.4">
-      <c r="C13" s="100" t="s">
+      <c r="C13" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="101"/>
-      <c r="E13" s="101"/>
-      <c r="F13" s="102"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="39"/>
     </row>
     <row r="14" spans="1:7" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C14" s="103"/>
-      <c r="D14" s="104"/>
-      <c r="E14" s="104"/>
-      <c r="F14" s="105"/>
+      <c r="C14" s="154"/>
+      <c r="D14" s="155"/>
+      <c r="E14" s="155"/>
+      <c r="F14" s="156"/>
     </row>
     <row r="15" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="69"/>
-      <c r="C15" s="113" t="str">
+      <c r="B15" s="128"/>
+      <c r="C15" s="131" t="str">
         <f>CONCATENATE("Total Amount Request for Approval (Revision"," ",D7,")")</f>
         <v>Total Amount Request for Approval (Revision 0)</v>
       </c>
-      <c r="D15" s="114">
+      <c r="D15" s="130">
         <f>'Cover Page'!E11</f>
         <v>0</v>
       </c>
-      <c r="E15" s="115"/>
-      <c r="F15" s="116"/>
+      <c r="E15" s="129"/>
     </row>
     <row r="16" spans="1:7" ht="1.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C16" s="117"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="119"/>
+      <c r="C16" s="111"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="112"/>
+      <c r="F16" s="113"/>
     </row>
     <row r="17" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C17" s="120"/>
-      <c r="D17" s="121" t="s">
+      <c r="C17" s="72"/>
+      <c r="D17" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="121" t="s">
+      <c r="E17" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="122" t="s">
+      <c r="F17" s="74" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="3:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C18" s="123"/>
-      <c r="D18" s="124"/>
-      <c r="E18" s="124"/>
-      <c r="F18" s="125"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="69"/>
     </row>
     <row r="19" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C19" s="123" t="str">
+      <c r="C19" s="41" t="str">
         <f>IF(D5&gt;0,"Subtotal Price:*","Estimated Subtotal Price:*")</f>
         <v>Estimated Subtotal Price:*</v>
       </c>
-      <c r="D19" s="124"/>
-      <c r="E19" s="124"/>
-      <c r="F19" s="125"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="69"/>
     </row>
     <row r="20" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C20" s="123" t="str">
+      <c r="C20" s="41" t="str">
         <f>IF($F$7="S","PST Cost (if excluded supplier from quote):",IF($F$7="M","Additional Warranty Cost (If applicable):","Rental Protection Insurance Cost:"))</f>
         <v>PST Cost (if excluded supplier from quote):</v>
       </c>
-      <c r="D20" s="124">
+      <c r="D20" s="68">
         <v>0</v>
       </c>
-      <c r="E20" s="124">
+      <c r="E20" s="68">
         <v>0</v>
       </c>
-      <c r="F20" s="125">
+      <c r="F20" s="69">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C21" s="123" t="str">
+      <c r="C21" s="41" t="str">
         <f>IF(OR($F$7="E",$F$7="S"),"Mobilization / Demob Cost (if excluded supplier from quote):","Freight (if excluded supplier from quote):")</f>
         <v>Mobilization / Demob Cost (if excluded supplier from quote):</v>
       </c>
-      <c r="D21" s="124">
+      <c r="D21" s="68">
         <v>0</v>
       </c>
-      <c r="E21" s="124">
+      <c r="E21" s="68">
         <v>0</v>
       </c>
-      <c r="F21" s="125">
+      <c r="F21" s="69">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C22" s="123" t="str">
+      <c r="C22" s="41" t="str">
         <f>IF($F$7="S","Site Orientation Cost (if excluded supplier from quote):",IF($F$7="M","Environmental Fees (if excluded supplier from quote):","Equipment Disinfection Cost if Out of Province Rental:"))</f>
         <v>Site Orientation Cost (if excluded supplier from quote):</v>
       </c>
-      <c r="D22" s="124">
+      <c r="D22" s="68">
         <v>0</v>
       </c>
-      <c r="E22" s="124">
+      <c r="E22" s="68">
         <v>0</v>
       </c>
-      <c r="F22" s="125">
+      <c r="F22" s="69">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="3:6" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C23" s="126" t="s">
+      <c r="C23" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="D23" s="127">
+      <c r="D23" s="70">
         <v>0</v>
       </c>
-      <c r="E23" s="127">
+      <c r="E23" s="70">
         <v>0</v>
       </c>
-      <c r="F23" s="128">
+      <c r="F23" s="71">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C24" s="120" t="s">
+      <c r="C24" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="129">
+      <c r="D24" s="87">
         <f>SUM(D19:D23)</f>
         <v>0</v>
       </c>
-      <c r="E24" s="129">
+      <c r="E24" s="87">
         <f>SUM(E19:E23)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="130">
+      <c r="F24" s="88">
         <f>SUM(F19:F23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C25" s="123" t="s">
+      <c r="C25" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="131">
+      <c r="D25" s="89">
         <v>0</v>
       </c>
-      <c r="E25" s="131">
+      <c r="E25" s="89">
         <v>0</v>
       </c>
-      <c r="F25" s="132">
+      <c r="F25" s="90">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="3:6" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C26" s="126" t="s">
+      <c r="C26" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="133">
+      <c r="D26" s="34">
         <f>D24*D25</f>
         <v>0</v>
       </c>
-      <c r="E26" s="133">
+      <c r="E26" s="34">
         <f>E24*E25</f>
         <v>0</v>
       </c>
-      <c r="F26" s="134">
+      <c r="F26" s="49">
         <f>F24*F25</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="3:6" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C27" s="135" t="s">
+      <c r="C27" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="136">
+      <c r="D27" s="53">
         <f>D26+D24</f>
         <v>0</v>
       </c>
-      <c r="E27" s="136">
+      <c r="E27" s="53">
         <f>E26+E24</f>
         <v>0</v>
       </c>
-      <c r="F27" s="137">
+      <c r="F27" s="54">
         <f>F26+F24</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="3:6" ht="1.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="117"/>
-      <c r="D28" s="118"/>
-      <c r="E28" s="118"/>
-      <c r="F28" s="119"/>
+      <c r="C28" s="111"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="112"/>
+      <c r="F28" s="113"/>
     </row>
     <row r="29" spans="3:6" ht="22.15" x14ac:dyDescent="0.4">
-      <c r="C29" s="138" t="s">
+      <c r="C29" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="D29" s="139"/>
-      <c r="E29" s="139"/>
-      <c r="F29" s="140"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="50"/>
     </row>
     <row r="30" spans="3:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="141"/>
-      <c r="D30" s="142"/>
-      <c r="E30" s="142"/>
-      <c r="F30" s="143"/>
+      <c r="C30" s="157"/>
+      <c r="D30" s="158"/>
+      <c r="E30" s="158"/>
+      <c r="F30" s="159"/>
     </row>
     <row r="31" spans="3:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C31" s="138" t="s">
+      <c r="C31" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="D31" s="144"/>
-      <c r="E31" s="144"/>
-      <c r="F31" s="145"/>
+      <c r="D31" s="145"/>
+      <c r="E31" s="145"/>
+      <c r="F31" s="146"/>
     </row>
     <row r="32" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C32" s="146" t="s">
+      <c r="C32" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="147">
+      <c r="D32" s="100">
         <f>D27</f>
         <v>0</v>
       </c>
-      <c r="E32" s="147">
+      <c r="E32" s="101">
         <f>E27</f>
         <v>0</v>
       </c>
-      <c r="F32" s="148">
+      <c r="F32" s="102">
         <f>F27</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C33" s="149" t="s">
+      <c r="C33" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="150" t="s">
+      <c r="D33" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="150" t="s">
+      <c r="E33" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="F33" s="151" t="s">
+      <c r="F33" s="77" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="34" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C34" s="149" t="s">
+      <c r="C34" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="150" t="s">
+      <c r="D34" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="E34" s="150" t="s">
+      <c r="E34" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="F34" s="151" t="s">
+      <c r="F34" s="77" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="35" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C35" s="149" t="s">
+      <c r="C35" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="150" t="s">
+      <c r="D35" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="E35" s="150" t="s">
+      <c r="E35" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="151" t="s">
+      <c r="F35" s="77" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="36" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C36" s="149" t="s">
+      <c r="C36" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="D36" s="150" t="s">
+      <c r="D36" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="E36" s="150" t="s">
+      <c r="E36" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="151" t="s">
+      <c r="F36" s="77" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="37" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C37" s="149" t="s">
+      <c r="C37" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="150" t="s">
+      <c r="D37" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="E37" s="150"/>
-      <c r="F37" s="151"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="77"/>
     </row>
     <row r="38" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C38" s="123" t="s">
+      <c r="C38" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="D38" s="152"/>
-      <c r="E38" s="153"/>
-      <c r="F38" s="145"/>
+      <c r="D38" s="93"/>
+      <c r="E38" s="149"/>
+      <c r="F38" s="150"/>
     </row>
     <row r="39" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C39" s="123" t="s">
+      <c r="C39" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="D39" s="139" t="s">
+      <c r="D39" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="E39" s="139"/>
-      <c r="F39" s="140"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="50"/>
     </row>
     <row r="40" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C40" s="123"/>
-      <c r="D40" s="139" t="s">
+      <c r="C40" s="41"/>
+      <c r="D40" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="E40" s="139"/>
-      <c r="F40" s="140"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="50"/>
     </row>
     <row r="41" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C41" s="123"/>
-      <c r="D41" s="139" t="s">
+      <c r="C41" s="41"/>
+      <c r="D41" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="E41" s="139"/>
-      <c r="F41" s="140"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="50"/>
     </row>
     <row r="42" spans="3:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="C42" s="123"/>
-      <c r="D42" s="139" t="s">
+      <c r="C42" s="41"/>
+      <c r="D42" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="E42" s="139"/>
-      <c r="F42" s="140"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="50"/>
     </row>
     <row r="43" spans="3:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C43" s="92" t="s">
+      <c r="C43" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="154"/>
-      <c r="E43" s="154"/>
-      <c r="F43" s="155"/>
+      <c r="D43" s="147"/>
+      <c r="E43" s="147"/>
+      <c r="F43" s="148"/>
     </row>
     <row r="44" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C44" s="149" t="s">
+      <c r="C44" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="124">
+      <c r="D44" s="76">
         <v>0</v>
       </c>
-      <c r="E44" s="124"/>
-      <c r="F44" s="125"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="69"/>
     </row>
     <row r="45" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C45" s="149" t="s">
+      <c r="C45" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="150" t="s">
+      <c r="D45" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="E45" s="150" t="s">
+      <c r="E45" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="F45" s="151" t="s">
+      <c r="F45" s="77" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="46" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C46" s="149" t="s">
+      <c r="C46" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="150" t="s">
+      <c r="D46" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="E46" s="150" t="s">
+      <c r="E46" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="F46" s="151" t="s">
+      <c r="F46" s="77" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="47" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C47" s="149" t="s">
+      <c r="C47" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="150" t="s">
+      <c r="D47" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="E47" s="150" t="s">
+      <c r="E47" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="151" t="s">
+      <c r="F47" s="77" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="48" spans="3:6" ht="15" x14ac:dyDescent="0.35">
-      <c r="C48" s="149" t="s">
+      <c r="C48" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="D48" s="150" t="s">
+      <c r="D48" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="E48" s="150" t="s">
+      <c r="E48" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="F48" s="151" t="s">
+      <c r="F48" s="77" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="49" spans="3:8" ht="15" x14ac:dyDescent="0.35">
-      <c r="C49" s="149" t="s">
+      <c r="C49" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="150" t="s">
+      <c r="D49" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="E49" s="150"/>
-      <c r="F49" s="151"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="77"/>
     </row>
     <row r="50" spans="3:8" ht="1.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C50" s="117"/>
-      <c r="D50" s="118"/>
-      <c r="E50" s="118"/>
-      <c r="F50" s="119"/>
+      <c r="C50" s="111"/>
+      <c r="D50" s="112"/>
+      <c r="E50" s="112"/>
+      <c r="F50" s="113"/>
     </row>
     <row r="51" spans="3:8" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C51" s="92" t="s">
+      <c r="C51" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="D51" s="154"/>
-      <c r="E51" s="154"/>
-      <c r="F51" s="155"/>
+      <c r="D51" s="147"/>
+      <c r="E51" s="147"/>
+      <c r="F51" s="148"/>
     </row>
     <row r="52" spans="3:8" ht="15" x14ac:dyDescent="0.35">
-      <c r="C52" s="149" t="s">
+      <c r="C52" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="D52" s="124">
+      <c r="D52" s="76">
         <v>0</v>
       </c>
-      <c r="E52" s="124"/>
-      <c r="F52" s="125"/>
+      <c r="E52" s="68"/>
+      <c r="F52" s="69"/>
     </row>
     <row r="53" spans="3:8" ht="15" x14ac:dyDescent="0.35">
-      <c r="C53" s="149" t="s">
+      <c r="C53" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="150" t="s">
+      <c r="D53" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="E53" s="150" t="s">
+      <c r="E53" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="F53" s="151" t="s">
+      <c r="F53" s="77" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="54" spans="3:8" ht="15" x14ac:dyDescent="0.35">
-      <c r="C54" s="149" t="s">
+      <c r="C54" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="D54" s="150" t="s">
+      <c r="D54" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="E54" s="150" t="s">
+      <c r="E54" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="F54" s="151" t="s">
+      <c r="F54" s="77" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="55" spans="3:8" ht="15" x14ac:dyDescent="0.35">
-      <c r="C55" s="149" t="s">
+      <c r="C55" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="D55" s="150" t="s">
+      <c r="D55" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="E55" s="150" t="s">
+      <c r="E55" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="F55" s="151" t="s">
+      <c r="F55" s="77" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="56" spans="3:8" ht="15" x14ac:dyDescent="0.35">
-      <c r="C56" s="149" t="s">
+      <c r="C56" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="D56" s="150" t="s">
+      <c r="D56" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="E56" s="150" t="s">
+      <c r="E56" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="F56" s="151" t="s">
+      <c r="F56" s="77" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="57" spans="3:8" ht="15.4" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C57" s="156" t="s">
+      <c r="C57" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="157" t="s">
+      <c r="D57" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="E57" s="157"/>
-      <c r="F57" s="158"/>
+      <c r="E57" s="79"/>
+      <c r="F57" s="80"/>
     </row>
     <row r="58" spans="3:8" ht="1.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C58" s="117"/>
-      <c r="D58" s="118"/>
-      <c r="E58" s="118"/>
-      <c r="F58" s="119"/>
+      <c r="C58" s="111"/>
+      <c r="D58" s="112"/>
+      <c r="E58" s="112"/>
+      <c r="F58" s="113"/>
     </row>
     <row r="59" spans="3:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C59" s="120" t="s">
+      <c r="C59" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="D59" s="159"/>
-      <c r="E59" s="159"/>
-      <c r="F59" s="160"/>
+      <c r="D59" s="81"/>
+      <c r="E59" s="81"/>
+      <c r="F59" s="82"/>
     </row>
     <row r="60" spans="3:8" ht="15" x14ac:dyDescent="0.4">
-      <c r="C60" s="123" t="s">
+      <c r="C60" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="D60" s="150"/>
-      <c r="E60" s="150" t="s">
+      <c r="D60" s="56"/>
+      <c r="E60" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="F60" s="161">
+      <c r="F60" s="83">
         <f ca="1">TODAY()</f>
-        <v>44108</v>
+        <v>44094</v>
       </c>
     </row>
     <row r="61" spans="3:8" ht="15" x14ac:dyDescent="0.4">
-      <c r="C61" s="123" t="s">
+      <c r="C61" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="D61" s="150"/>
-      <c r="E61" s="150" t="s">
+      <c r="D61" s="56"/>
+      <c r="E61" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="F61" s="161"/>
+      <c r="F61" s="83"/>
     </row>
     <row r="62" spans="3:8" ht="15.4" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C62" s="60"/>
-      <c r="D62" s="61" t="s">
+      <c r="C62" s="116"/>
+      <c r="D62" s="119" t="s">
         <v>104</v>
       </c>
-      <c r="E62" s="62" t="s">
+      <c r="E62" s="120" t="s">
         <v>105</v>
       </c>
-      <c r="F62" s="63" t="s">
+      <c r="F62" s="121" t="s">
         <v>106</v>
       </c>
-      <c r="G62" s="34"/>
-      <c r="H62" s="34"/>
+      <c r="G62" s="45"/>
+      <c r="H62" s="45"/>
     </row>
     <row r="63" spans="3:8" ht="23" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C63" s="64" t="s">
+      <c r="C63" s="122" t="s">
         <v>123</v>
       </c>
-      <c r="D63" s="68"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="66"/>
-      <c r="G63" s="35"/>
-      <c r="H63" s="35"/>
+      <c r="D63" s="127"/>
+      <c r="E63" s="81"/>
+      <c r="F63" s="124"/>
+      <c r="G63" s="46"/>
+      <c r="H63" s="46"/>
     </row>
     <row r="64" spans="3:8" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C64" s="59" t="s">
+      <c r="C64" s="115" t="s">
         <v>124</v>
       </c>
-      <c r="D64" s="83"/>
-      <c r="E64" s="84"/>
-      <c r="F64" s="85"/>
+      <c r="D64" s="142"/>
+      <c r="E64" s="143"/>
+      <c r="F64" s="144"/>
     </row>
     <row r="65" spans="1:8" ht="23" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="36">
+      <c r="A65" s="47">
         <v>10000</v>
       </c>
-      <c r="B65" s="36"/>
-      <c r="C65" s="65" t="str">
+      <c r="B65" s="47"/>
+      <c r="C65" s="123" t="str">
         <f>IF(OR($D$27&gt;$A$65,$E$27&gt;$A$65,$F$27&gt;$A$65),"Client Maury Simoneau (Up to $50,000.00)"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D65" s="68"/>
-      <c r="E65" s="46"/>
-      <c r="F65" s="66"/>
-      <c r="G65" s="35"/>
-      <c r="H65" s="35"/>
+      <c r="D65" s="127"/>
+      <c r="E65" s="81"/>
+      <c r="F65" s="124"/>
+      <c r="G65" s="46"/>
+      <c r="H65" s="46"/>
     </row>
     <row r="66" spans="1:8" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C66" s="58" t="str">
+      <c r="C66" s="114" t="str">
         <f>IF(OR($D$27&gt;$A$65,$E$27&gt;$A$65,$F$27&gt;$A$65),"Comment from Maury Simoneau (If Applicable):"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D66" s="83"/>
-      <c r="E66" s="84"/>
-      <c r="F66" s="85"/>
+      <c r="D66" s="142"/>
+      <c r="E66" s="143"/>
+      <c r="F66" s="144"/>
     </row>
     <row r="67" spans="1:8" ht="23" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="36">
+      <c r="A67" s="47">
         <v>50000</v>
       </c>
-      <c r="B67" s="36"/>
-      <c r="C67" s="65" t="str">
+      <c r="B67" s="47"/>
+      <c r="C67" s="123" t="str">
         <f>IF(OR($D$27&gt;$A$67,$E$27&gt;$A$67,$F$27&gt;$A$67),"Client Chris Whorton (+$50,000.00)"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D67" s="68"/>
-      <c r="E67" s="46"/>
-      <c r="F67" s="66"/>
-      <c r="G67" s="35"/>
-      <c r="H67" s="35"/>
+      <c r="D67" s="127"/>
+      <c r="E67" s="81"/>
+      <c r="F67" s="124"/>
+      <c r="G67" s="46"/>
+      <c r="H67" s="46"/>
     </row>
     <row r="68" spans="1:8" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C68" s="59" t="str">
+      <c r="C68" s="115" t="str">
         <f>IF(OR($D$27&gt;$A$67,$E$27&gt;$A$67,$F$27&gt;$A$67),"Comment from Chris Whorton (If Applicable):"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D68" s="83"/>
-      <c r="E68" s="84"/>
-      <c r="F68" s="85"/>
+      <c r="D68" s="142"/>
+      <c r="E68" s="143"/>
+      <c r="F68" s="144"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C69" s="33"/>
@@ -5451,6 +5469,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C8:F8"/>
     <mergeCell ref="D64:F64"/>
     <mergeCell ref="D66:F66"/>
     <mergeCell ref="D68:F68"/>
@@ -5458,11 +5481,6 @@
     <mergeCell ref="D43:F43"/>
     <mergeCell ref="D51:F51"/>
     <mergeCell ref="E38:F38"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C8:F8"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>